<commit_message>
few tweaks and updated results and data
</commit_message>
<xml_diff>
--- a/Output/GM.xlsx
+++ b/Output/GM.xlsx
@@ -539,17 +539,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>98.0 (4)</t>
+          <t>872.0 (11)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>363.5 (7)</t>
+          <t>750.5 (11)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>265.5 (3)</t>
+          <t>121.5 (0)</t>
         </is>
       </c>
     </row>
@@ -567,17 +567,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>134.0 (9)</t>
+          <t>857.0 (27)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>383.0 (9)</t>
+          <t>744.5 (18)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>249.0 (0)</t>
+          <t>112.5 (9)</t>
         </is>
       </c>
     </row>
@@ -595,17 +595,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>56.0 (12)</t>
+          <t>587.0 (36)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>281.0 (10)</t>
+          <t>546.5 (22)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>225.0 (-2)</t>
+          <t>40.5 (14)</t>
         </is>
       </c>
     </row>
@@ -627,17 +627,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>164.0 (7)</t>
+          <t>1084.0 (15)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>449.5 (11)</t>
+          <t>909.5 (15)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>285.5 (4)</t>
+          <t>174.5 (0)</t>
         </is>
       </c>
     </row>
@@ -655,17 +655,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>305.0 (13)</t>
+          <t>1282.0 (33)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>509.5 (18)</t>
+          <t>998.0 (28)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>204.5 (5)</t>
+          <t>284.0 (5)</t>
         </is>
       </c>
     </row>
@@ -683,17 +683,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>327.0 (13)</t>
+          <t>1355.0 (32)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>395.0 (14)</t>
+          <t>909.0 (23)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>68.0 (1)</t>
+          <t>446.0 (8)</t>
         </is>
       </c>
     </row>
@@ -715,17 +715,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>118.0 (7)</t>
+          <t>931.0 (18)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>422.5 (5)</t>
+          <t>829.0 (11)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>304.5 (-1)</t>
+          <t>102.0 (7)</t>
         </is>
       </c>
     </row>
@@ -743,17 +743,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>119.0 (14)</t>
+          <t>838.0 (36)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>413.0 (10)</t>
+          <t>772.5 (21)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>294.0 (-4)</t>
+          <t>65.5 (15)</t>
         </is>
       </c>
     </row>
@@ -771,17 +771,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>134.0 (26)</t>
+          <t>792.0 (64)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>321.5 (16)</t>
+          <t>650.5 (35)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>187.5 (-10)</t>
+          <t>141.5 (29)</t>
         </is>
       </c>
     </row>

</xml_diff>